<commit_message>
lots of changes: regulator layout improved bom minimized inner top layer completely gnd UB single pole pullups for use without pi swiched to new kicad version and fp lib motor and servo netanmes fixed added input filtering
</commit_message>
<xml_diff>
--- a/Doc/BOM.xlsx
+++ b/Doc/BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="291">
   <si>
     <t xml:space="preserve">Ref.Des.</t>
   </si>
@@ -57,154 +57,142 @@
     <t xml:space="preserve">notes</t>
   </si>
   <si>
-    <t xml:space="preserve">R1</t>
+    <t xml:space="preserve">R7</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">470k</t>
+    <t xml:space="preserve">2k4</t>
   </si>
   <si>
     <t xml:space="preserve">0603</t>
   </si>
   <si>
+    <t xml:space="preserve">Yageo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603JR-072K4L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603JR-072K4L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exact part my be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0782KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-0782KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R11, R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603JR-07180KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603JR-07180KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0747KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-0747KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6, R10, R21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0712KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-0712KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12, R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0734KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-0734KL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5k1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-075K1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-075K1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2,R3,R4,R5,R32,R40,R41,R43,R44,R45,R46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1k6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-071K6L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-071K6L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R47,R48,R49,R50,R51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-07330RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603FR-07330RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0R1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Panasonic</t>
   </si>
   <si>
-    <t xml:space="preserve">ERJ-PA3J474V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mouser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-PA3J474V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exact part my be changed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2k4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yageo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603JR-072K4L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603JR-072K4L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0782KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-0782KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R11, R23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0743KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-0743KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0747KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-0747KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6, R10, R21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0712KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-0712KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12, R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8k2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-078K2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-078K2L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5k1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-075K1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-075K1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2,R3,R4,R5,R32,R40,R41,R43,R44,R45,R46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1k6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-071K6L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-071K6L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R47,R48,R49,R50,R51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-07330RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-07330RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0R1</t>
-  </si>
-  <si>
     <t xml:space="preserve">ERJ-3RSFR10V</t>
   </si>
   <si>
     <t xml:space="preserve">667-ERJ-3RSFR10V</t>
   </si>
   <si>
-    <t xml:space="preserve">C13</t>
+    <t xml:space="preserve">C16, C24</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitor</t>
@@ -225,39 +213,15 @@
     <t xml:space="preserve">81-GRM31CR60J107ME9L</t>
   </si>
   <si>
-    <t xml:space="preserve">C24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47µF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM31CR61A476KE15L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81-GRM31CR61A476KE5L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22µF</t>
+    <t xml:space="preserve">C10, C11, C12, C20, C30, C34, C52, C54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10µF</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;24V</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM32ER61E226KE15L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81-GRM32ER61E226KE15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C20, C30, C34, C52, C54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10µF</t>
-  </si>
-  <si>
     <t xml:space="preserve">GRM188R6YA106MA73D</t>
   </si>
   <si>
@@ -282,7 +246,7 @@
     <t xml:space="preserve">810-C1608X5R1V225K</t>
   </si>
   <si>
-    <t xml:space="preserve">C11, C12,C40,C51</t>
+    <t xml:space="preserve">C14, C15,C40,C51</t>
   </si>
   <si>
     <t xml:space="preserve">1µF</t>
@@ -294,7 +258,7 @@
     <t xml:space="preserve">81-GRM188R61E105KA12</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2,C23,C32,C33,C41,C42,C43,C44, C50,C53,C55,C61,C62,C63</t>
+    <t xml:space="preserve">C1,C2,C13,C23,C32,C33,C41,C42,C43,C44, C50,C53,C55,C61,C62,C63</t>
   </si>
   <si>
     <t xml:space="preserve">100nF</t>
@@ -570,7 +534,7 @@
     <t xml:space="preserve">78-SISS27DN-T1-GE3</t>
   </si>
   <si>
-    <t xml:space="preserve">Better Alternative: SISS27ADN-T1-GE3</t>
+    <t xml:space="preserve">better:: SISS27ADN-T1-GE3</t>
   </si>
   <si>
     <t xml:space="preserve">Q2</t>
@@ -594,13 +558,13 @@
     <t xml:space="preserve">N-MOSFET</t>
   </si>
   <si>
-    <t xml:space="preserve">SI7114ADN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">781-SI7114ADN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative: SI7114DN-T1-E3</t>
+    <t xml:space="preserve">SIS434DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">781-SIS434DN-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">better: SIS862DN-T1-GE3</t>
   </si>
   <si>
     <t xml:space="preserve">U10</t>
@@ -747,7 +711,7 @@
     <t xml:space="preserve">131-4776</t>
   </si>
   <si>
-    <t xml:space="preserve">type alternative</t>
+    <t xml:space="preserve">combined (preffered)</t>
   </si>
   <si>
     <t xml:space="preserve">note</t>
@@ -1049,16 +1013,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1102,25 +1066,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:54"/>
+  <dimension ref="1:51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="53.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.3076923076923"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.6032388663968"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1161,16 +1125,15 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
@@ -2185,1112 +2148,109 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+    <row r="3" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="0"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
-      <c r="P3" s="0"/>
-      <c r="Q3" s="0"/>
-      <c r="R3" s="0"/>
-      <c r="S3" s="0"/>
-      <c r="T3" s="0"/>
-      <c r="U3" s="0"/>
-      <c r="V3" s="0"/>
-      <c r="W3" s="0"/>
-      <c r="X3" s="0"/>
-      <c r="Y3" s="0"/>
-      <c r="Z3" s="0"/>
-      <c r="AA3" s="0"/>
-      <c r="AB3" s="0"/>
-      <c r="AC3" s="0"/>
-      <c r="AD3" s="0"/>
-      <c r="AE3" s="0"/>
-      <c r="AF3" s="0"/>
-      <c r="AG3" s="0"/>
-      <c r="AH3" s="0"/>
-      <c r="AI3" s="0"/>
-      <c r="AJ3" s="0"/>
-      <c r="AK3" s="0"/>
-      <c r="AL3" s="0"/>
-      <c r="AM3" s="0"/>
-      <c r="AN3" s="0"/>
-      <c r="AO3" s="0"/>
-      <c r="AP3" s="0"/>
-      <c r="AQ3" s="0"/>
-      <c r="AR3" s="0"/>
-      <c r="AS3" s="0"/>
-      <c r="AT3" s="0"/>
-      <c r="AU3" s="0"/>
-      <c r="AV3" s="0"/>
-      <c r="AW3" s="0"/>
-      <c r="AX3" s="0"/>
-      <c r="AY3" s="0"/>
-      <c r="AZ3" s="0"/>
-      <c r="BA3" s="0"/>
-      <c r="BB3" s="0"/>
-      <c r="BC3" s="0"/>
-      <c r="BD3" s="0"/>
-      <c r="BE3" s="0"/>
-      <c r="BF3" s="0"/>
-      <c r="BG3" s="0"/>
-      <c r="BH3" s="0"/>
-      <c r="BI3" s="0"/>
-      <c r="BJ3" s="0"/>
-      <c r="BK3" s="0"/>
-      <c r="BL3" s="0"/>
-      <c r="BM3" s="0"/>
-      <c r="BN3" s="0"/>
-      <c r="BO3" s="0"/>
-      <c r="BP3" s="0"/>
-      <c r="BQ3" s="0"/>
-      <c r="BR3" s="0"/>
-      <c r="BS3" s="0"/>
-      <c r="BT3" s="0"/>
-      <c r="BU3" s="0"/>
-      <c r="BV3" s="0"/>
-      <c r="BW3" s="0"/>
-      <c r="BX3" s="0"/>
-      <c r="BY3" s="0"/>
-      <c r="BZ3" s="0"/>
-      <c r="CA3" s="0"/>
-      <c r="CB3" s="0"/>
-      <c r="CC3" s="0"/>
-      <c r="CD3" s="0"/>
-      <c r="CE3" s="0"/>
-      <c r="CF3" s="0"/>
-      <c r="CG3" s="0"/>
-      <c r="CH3" s="0"/>
-      <c r="CI3" s="0"/>
-      <c r="CJ3" s="0"/>
-      <c r="CK3" s="0"/>
-      <c r="CL3" s="0"/>
-      <c r="CM3" s="0"/>
-      <c r="CN3" s="0"/>
-      <c r="CO3" s="0"/>
-      <c r="CP3" s="0"/>
-      <c r="CQ3" s="0"/>
-      <c r="CR3" s="0"/>
-      <c r="CS3" s="0"/>
-      <c r="CT3" s="0"/>
-      <c r="CU3" s="0"/>
-      <c r="CV3" s="0"/>
-      <c r="CW3" s="0"/>
-      <c r="CX3" s="0"/>
-      <c r="CY3" s="0"/>
-      <c r="CZ3" s="0"/>
-      <c r="DA3" s="0"/>
-      <c r="DB3" s="0"/>
-      <c r="DC3" s="0"/>
-      <c r="DD3" s="0"/>
-      <c r="DE3" s="0"/>
-      <c r="DF3" s="0"/>
-      <c r="DG3" s="0"/>
-      <c r="DH3" s="0"/>
-      <c r="DI3" s="0"/>
-      <c r="DJ3" s="0"/>
-      <c r="DK3" s="0"/>
-      <c r="DL3" s="0"/>
-      <c r="DM3" s="0"/>
-      <c r="DN3" s="0"/>
-      <c r="DO3" s="0"/>
-      <c r="DP3" s="0"/>
-      <c r="DQ3" s="0"/>
-      <c r="DR3" s="0"/>
-      <c r="DS3" s="0"/>
-      <c r="DT3" s="0"/>
-      <c r="DU3" s="0"/>
-      <c r="DV3" s="0"/>
-      <c r="DW3" s="0"/>
-      <c r="DX3" s="0"/>
-      <c r="DY3" s="0"/>
-      <c r="DZ3" s="0"/>
-      <c r="EA3" s="0"/>
-      <c r="EB3" s="0"/>
-      <c r="EC3" s="0"/>
-      <c r="ED3" s="0"/>
-      <c r="EE3" s="0"/>
-      <c r="EF3" s="0"/>
-      <c r="EG3" s="0"/>
-      <c r="EH3" s="0"/>
-      <c r="EI3" s="0"/>
-      <c r="EJ3" s="0"/>
-      <c r="EK3" s="0"/>
-      <c r="EL3" s="0"/>
-      <c r="EM3" s="0"/>
-      <c r="EN3" s="0"/>
-      <c r="EO3" s="0"/>
-      <c r="EP3" s="0"/>
-      <c r="EQ3" s="0"/>
-      <c r="ER3" s="0"/>
-      <c r="ES3" s="0"/>
-      <c r="ET3" s="0"/>
-      <c r="EU3" s="0"/>
-      <c r="EV3" s="0"/>
-      <c r="EW3" s="0"/>
-      <c r="EX3" s="0"/>
-      <c r="EY3" s="0"/>
-      <c r="EZ3" s="0"/>
-      <c r="FA3" s="0"/>
-      <c r="FB3" s="0"/>
-      <c r="FC3" s="0"/>
-      <c r="FD3" s="0"/>
-      <c r="FE3" s="0"/>
-      <c r="FF3" s="0"/>
-      <c r="FG3" s="0"/>
-      <c r="FH3" s="0"/>
-      <c r="FI3" s="0"/>
-      <c r="FJ3" s="0"/>
-      <c r="FK3" s="0"/>
-      <c r="FL3" s="0"/>
-      <c r="FM3" s="0"/>
-      <c r="FN3" s="0"/>
-      <c r="FO3" s="0"/>
-      <c r="FP3" s="0"/>
-      <c r="FQ3" s="0"/>
-      <c r="FR3" s="0"/>
-      <c r="FS3" s="0"/>
-      <c r="FT3" s="0"/>
-      <c r="FU3" s="0"/>
-      <c r="FV3" s="0"/>
-      <c r="FW3" s="0"/>
-      <c r="FX3" s="0"/>
-      <c r="FY3" s="0"/>
-      <c r="FZ3" s="0"/>
-      <c r="GA3" s="0"/>
-      <c r="GB3" s="0"/>
-      <c r="GC3" s="0"/>
-      <c r="GD3" s="0"/>
-      <c r="GE3" s="0"/>
-      <c r="GF3" s="0"/>
-      <c r="GG3" s="0"/>
-      <c r="GH3" s="0"/>
-      <c r="GI3" s="0"/>
-      <c r="GJ3" s="0"/>
-      <c r="GK3" s="0"/>
-      <c r="GL3" s="0"/>
-      <c r="GM3" s="0"/>
-      <c r="GN3" s="0"/>
-      <c r="GO3" s="0"/>
-      <c r="GP3" s="0"/>
-      <c r="GQ3" s="0"/>
-      <c r="GR3" s="0"/>
-      <c r="GS3" s="0"/>
-      <c r="GT3" s="0"/>
-      <c r="GU3" s="0"/>
-      <c r="GV3" s="0"/>
-      <c r="GW3" s="0"/>
-      <c r="GX3" s="0"/>
-      <c r="GY3" s="0"/>
-      <c r="GZ3" s="0"/>
-      <c r="HA3" s="0"/>
-      <c r="HB3" s="0"/>
-      <c r="HC3" s="0"/>
-      <c r="HD3" s="0"/>
-      <c r="HE3" s="0"/>
-      <c r="HF3" s="0"/>
-      <c r="HG3" s="0"/>
-      <c r="HH3" s="0"/>
-      <c r="HI3" s="0"/>
-      <c r="HJ3" s="0"/>
-      <c r="HK3" s="0"/>
-      <c r="HL3" s="0"/>
-      <c r="HM3" s="0"/>
-      <c r="HN3" s="0"/>
-      <c r="HO3" s="0"/>
-      <c r="HP3" s="0"/>
-      <c r="HQ3" s="0"/>
-      <c r="HR3" s="0"/>
-      <c r="HS3" s="0"/>
-      <c r="HT3" s="0"/>
-      <c r="HU3" s="0"/>
-      <c r="HV3" s="0"/>
-      <c r="HW3" s="0"/>
-      <c r="HX3" s="0"/>
-      <c r="HY3" s="0"/>
-      <c r="HZ3" s="0"/>
-      <c r="IA3" s="0"/>
-      <c r="IB3" s="0"/>
-      <c r="IC3" s="0"/>
-      <c r="ID3" s="0"/>
-      <c r="IE3" s="0"/>
-      <c r="IF3" s="0"/>
-      <c r="IG3" s="0"/>
-      <c r="IH3" s="0"/>
-      <c r="II3" s="0"/>
-      <c r="IJ3" s="0"/>
-      <c r="IK3" s="0"/>
-      <c r="IL3" s="0"/>
-      <c r="IM3" s="0"/>
-      <c r="IN3" s="0"/>
-      <c r="IO3" s="0"/>
-      <c r="IP3" s="0"/>
-      <c r="IQ3" s="0"/>
-      <c r="IR3" s="0"/>
-      <c r="IS3" s="0"/>
-      <c r="IT3" s="0"/>
-      <c r="IU3" s="0"/>
-      <c r="IV3" s="0"/>
-      <c r="IW3" s="0"/>
-      <c r="IX3" s="0"/>
-      <c r="IY3" s="0"/>
-      <c r="IZ3" s="0"/>
-      <c r="JA3" s="0"/>
-      <c r="JB3" s="0"/>
-      <c r="JC3" s="0"/>
-      <c r="JD3" s="0"/>
-      <c r="JE3" s="0"/>
-      <c r="JF3" s="0"/>
-      <c r="JG3" s="0"/>
-      <c r="JH3" s="0"/>
-      <c r="JI3" s="0"/>
-      <c r="JJ3" s="0"/>
-      <c r="JK3" s="0"/>
-      <c r="JL3" s="0"/>
-      <c r="JM3" s="0"/>
-      <c r="JN3" s="0"/>
-      <c r="JO3" s="0"/>
-      <c r="JP3" s="0"/>
-      <c r="JQ3" s="0"/>
-      <c r="JR3" s="0"/>
-      <c r="JS3" s="0"/>
-      <c r="JT3" s="0"/>
-      <c r="JU3" s="0"/>
-      <c r="JV3" s="0"/>
-      <c r="JW3" s="0"/>
-      <c r="JX3" s="0"/>
-      <c r="JY3" s="0"/>
-      <c r="JZ3" s="0"/>
-      <c r="KA3" s="0"/>
-      <c r="KB3" s="0"/>
-      <c r="KC3" s="0"/>
-      <c r="KD3" s="0"/>
-      <c r="KE3" s="0"/>
-      <c r="KF3" s="0"/>
-      <c r="KG3" s="0"/>
-      <c r="KH3" s="0"/>
-      <c r="KI3" s="0"/>
-      <c r="KJ3" s="0"/>
-      <c r="KK3" s="0"/>
-      <c r="KL3" s="0"/>
-      <c r="KM3" s="0"/>
-      <c r="KN3" s="0"/>
-      <c r="KO3" s="0"/>
-      <c r="KP3" s="0"/>
-      <c r="KQ3" s="0"/>
-      <c r="KR3" s="0"/>
-      <c r="KS3" s="0"/>
-      <c r="KT3" s="0"/>
-      <c r="KU3" s="0"/>
-      <c r="KV3" s="0"/>
-      <c r="KW3" s="0"/>
-      <c r="KX3" s="0"/>
-      <c r="KY3" s="0"/>
-      <c r="KZ3" s="0"/>
-      <c r="LA3" s="0"/>
-      <c r="LB3" s="0"/>
-      <c r="LC3" s="0"/>
-      <c r="LD3" s="0"/>
-      <c r="LE3" s="0"/>
-      <c r="LF3" s="0"/>
-      <c r="LG3" s="0"/>
-      <c r="LH3" s="0"/>
-      <c r="LI3" s="0"/>
-      <c r="LJ3" s="0"/>
-      <c r="LK3" s="0"/>
-      <c r="LL3" s="0"/>
-      <c r="LM3" s="0"/>
-      <c r="LN3" s="0"/>
-      <c r="LO3" s="0"/>
-      <c r="LP3" s="0"/>
-      <c r="LQ3" s="0"/>
-      <c r="LR3" s="0"/>
-      <c r="LS3" s="0"/>
-      <c r="LT3" s="0"/>
-      <c r="LU3" s="0"/>
-      <c r="LV3" s="0"/>
-      <c r="LW3" s="0"/>
-      <c r="LX3" s="0"/>
-      <c r="LY3" s="0"/>
-      <c r="LZ3" s="0"/>
-      <c r="MA3" s="0"/>
-      <c r="MB3" s="0"/>
-      <c r="MC3" s="0"/>
-      <c r="MD3" s="0"/>
-      <c r="ME3" s="0"/>
-      <c r="MF3" s="0"/>
-      <c r="MG3" s="0"/>
-      <c r="MH3" s="0"/>
-      <c r="MI3" s="0"/>
-      <c r="MJ3" s="0"/>
-      <c r="MK3" s="0"/>
-      <c r="ML3" s="0"/>
-      <c r="MM3" s="0"/>
-      <c r="MN3" s="0"/>
-      <c r="MO3" s="0"/>
-      <c r="MP3" s="0"/>
-      <c r="MQ3" s="0"/>
-      <c r="MR3" s="0"/>
-      <c r="MS3" s="0"/>
-      <c r="MT3" s="0"/>
-      <c r="MU3" s="0"/>
-      <c r="MV3" s="0"/>
-      <c r="MW3" s="0"/>
-      <c r="MX3" s="0"/>
-      <c r="MY3" s="0"/>
-      <c r="MZ3" s="0"/>
-      <c r="NA3" s="0"/>
-      <c r="NB3" s="0"/>
-      <c r="NC3" s="0"/>
-      <c r="ND3" s="0"/>
-      <c r="NE3" s="0"/>
-      <c r="NF3" s="0"/>
-      <c r="NG3" s="0"/>
-      <c r="NH3" s="0"/>
-      <c r="NI3" s="0"/>
-      <c r="NJ3" s="0"/>
-      <c r="NK3" s="0"/>
-      <c r="NL3" s="0"/>
-      <c r="NM3" s="0"/>
-      <c r="NN3" s="0"/>
-      <c r="NO3" s="0"/>
-      <c r="NP3" s="0"/>
-      <c r="NQ3" s="0"/>
-      <c r="NR3" s="0"/>
-      <c r="NS3" s="0"/>
-      <c r="NT3" s="0"/>
-      <c r="NU3" s="0"/>
-      <c r="NV3" s="0"/>
-      <c r="NW3" s="0"/>
-      <c r="NX3" s="0"/>
-      <c r="NY3" s="0"/>
-      <c r="NZ3" s="0"/>
-      <c r="OA3" s="0"/>
-      <c r="OB3" s="0"/>
-      <c r="OC3" s="0"/>
-      <c r="OD3" s="0"/>
-      <c r="OE3" s="0"/>
-      <c r="OF3" s="0"/>
-      <c r="OG3" s="0"/>
-      <c r="OH3" s="0"/>
-      <c r="OI3" s="0"/>
-      <c r="OJ3" s="0"/>
-      <c r="OK3" s="0"/>
-      <c r="OL3" s="0"/>
-      <c r="OM3" s="0"/>
-      <c r="ON3" s="0"/>
-      <c r="OO3" s="0"/>
-      <c r="OP3" s="0"/>
-      <c r="OQ3" s="0"/>
-      <c r="OR3" s="0"/>
-      <c r="OS3" s="0"/>
-      <c r="OT3" s="0"/>
-      <c r="OU3" s="0"/>
-      <c r="OV3" s="0"/>
-      <c r="OW3" s="0"/>
-      <c r="OX3" s="0"/>
-      <c r="OY3" s="0"/>
-      <c r="OZ3" s="0"/>
-      <c r="PA3" s="0"/>
-      <c r="PB3" s="0"/>
-      <c r="PC3" s="0"/>
-      <c r="PD3" s="0"/>
-      <c r="PE3" s="0"/>
-      <c r="PF3" s="0"/>
-      <c r="PG3" s="0"/>
-      <c r="PH3" s="0"/>
-      <c r="PI3" s="0"/>
-      <c r="PJ3" s="0"/>
-      <c r="PK3" s="0"/>
-      <c r="PL3" s="0"/>
-      <c r="PM3" s="0"/>
-      <c r="PN3" s="0"/>
-      <c r="PO3" s="0"/>
-      <c r="PP3" s="0"/>
-      <c r="PQ3" s="0"/>
-      <c r="PR3" s="0"/>
-      <c r="PS3" s="0"/>
-      <c r="PT3" s="0"/>
-      <c r="PU3" s="0"/>
-      <c r="PV3" s="0"/>
-      <c r="PW3" s="0"/>
-      <c r="PX3" s="0"/>
-      <c r="PY3" s="0"/>
-      <c r="PZ3" s="0"/>
-      <c r="QA3" s="0"/>
-      <c r="QB3" s="0"/>
-      <c r="QC3" s="0"/>
-      <c r="QD3" s="0"/>
-      <c r="QE3" s="0"/>
-      <c r="QF3" s="0"/>
-      <c r="QG3" s="0"/>
-      <c r="QH3" s="0"/>
-      <c r="QI3" s="0"/>
-      <c r="QJ3" s="0"/>
-      <c r="QK3" s="0"/>
-      <c r="QL3" s="0"/>
-      <c r="QM3" s="0"/>
-      <c r="QN3" s="0"/>
-      <c r="QO3" s="0"/>
-      <c r="QP3" s="0"/>
-      <c r="QQ3" s="0"/>
-      <c r="QR3" s="0"/>
-      <c r="QS3" s="0"/>
-      <c r="QT3" s="0"/>
-      <c r="QU3" s="0"/>
-      <c r="QV3" s="0"/>
-      <c r="QW3" s="0"/>
-      <c r="QX3" s="0"/>
-      <c r="QY3" s="0"/>
-      <c r="QZ3" s="0"/>
-      <c r="RA3" s="0"/>
-      <c r="RB3" s="0"/>
-      <c r="RC3" s="0"/>
-      <c r="RD3" s="0"/>
-      <c r="RE3" s="0"/>
-      <c r="RF3" s="0"/>
-      <c r="RG3" s="0"/>
-      <c r="RH3" s="0"/>
-      <c r="RI3" s="0"/>
-      <c r="RJ3" s="0"/>
-      <c r="RK3" s="0"/>
-      <c r="RL3" s="0"/>
-      <c r="RM3" s="0"/>
-      <c r="RN3" s="0"/>
-      <c r="RO3" s="0"/>
-      <c r="RP3" s="0"/>
-      <c r="RQ3" s="0"/>
-      <c r="RR3" s="0"/>
-      <c r="RS3" s="0"/>
-      <c r="RT3" s="0"/>
-      <c r="RU3" s="0"/>
-      <c r="RV3" s="0"/>
-      <c r="RW3" s="0"/>
-      <c r="RX3" s="0"/>
-      <c r="RY3" s="0"/>
-      <c r="RZ3" s="0"/>
-      <c r="SA3" s="0"/>
-      <c r="SB3" s="0"/>
-      <c r="SC3" s="0"/>
-      <c r="SD3" s="0"/>
-      <c r="SE3" s="0"/>
-      <c r="SF3" s="0"/>
-      <c r="SG3" s="0"/>
-      <c r="SH3" s="0"/>
-      <c r="SI3" s="0"/>
-      <c r="SJ3" s="0"/>
-      <c r="SK3" s="0"/>
-      <c r="SL3" s="0"/>
-      <c r="SM3" s="0"/>
-      <c r="SN3" s="0"/>
-      <c r="SO3" s="0"/>
-      <c r="SP3" s="0"/>
-      <c r="SQ3" s="0"/>
-      <c r="SR3" s="0"/>
-      <c r="SS3" s="0"/>
-      <c r="ST3" s="0"/>
-      <c r="SU3" s="0"/>
-      <c r="SV3" s="0"/>
-      <c r="SW3" s="0"/>
-      <c r="SX3" s="0"/>
-      <c r="SY3" s="0"/>
-      <c r="SZ3" s="0"/>
-      <c r="TA3" s="0"/>
-      <c r="TB3" s="0"/>
-      <c r="TC3" s="0"/>
-      <c r="TD3" s="0"/>
-      <c r="TE3" s="0"/>
-      <c r="TF3" s="0"/>
-      <c r="TG3" s="0"/>
-      <c r="TH3" s="0"/>
-      <c r="TI3" s="0"/>
-      <c r="TJ3" s="0"/>
-      <c r="TK3" s="0"/>
-      <c r="TL3" s="0"/>
-      <c r="TM3" s="0"/>
-      <c r="TN3" s="0"/>
-      <c r="TO3" s="0"/>
-      <c r="TP3" s="0"/>
-      <c r="TQ3" s="0"/>
-      <c r="TR3" s="0"/>
-      <c r="TS3" s="0"/>
-      <c r="TT3" s="0"/>
-      <c r="TU3" s="0"/>
-      <c r="TV3" s="0"/>
-      <c r="TW3" s="0"/>
-      <c r="TX3" s="0"/>
-      <c r="TY3" s="0"/>
-      <c r="TZ3" s="0"/>
-      <c r="UA3" s="0"/>
-      <c r="UB3" s="0"/>
-      <c r="UC3" s="0"/>
-      <c r="UD3" s="0"/>
-      <c r="UE3" s="0"/>
-      <c r="UF3" s="0"/>
-      <c r="UG3" s="0"/>
-      <c r="UH3" s="0"/>
-      <c r="UI3" s="0"/>
-      <c r="UJ3" s="0"/>
-      <c r="UK3" s="0"/>
-      <c r="UL3" s="0"/>
-      <c r="UM3" s="0"/>
-      <c r="UN3" s="0"/>
-      <c r="UO3" s="0"/>
-      <c r="UP3" s="0"/>
-      <c r="UQ3" s="0"/>
-      <c r="UR3" s="0"/>
-      <c r="US3" s="0"/>
-      <c r="UT3" s="0"/>
-      <c r="UU3" s="0"/>
-      <c r="UV3" s="0"/>
-      <c r="UW3" s="0"/>
-      <c r="UX3" s="0"/>
-      <c r="UY3" s="0"/>
-      <c r="UZ3" s="0"/>
-      <c r="VA3" s="0"/>
-      <c r="VB3" s="0"/>
-      <c r="VC3" s="0"/>
-      <c r="VD3" s="0"/>
-      <c r="VE3" s="0"/>
-      <c r="VF3" s="0"/>
-      <c r="VG3" s="0"/>
-      <c r="VH3" s="0"/>
-      <c r="VI3" s="0"/>
-      <c r="VJ3" s="0"/>
-      <c r="VK3" s="0"/>
-      <c r="VL3" s="0"/>
-      <c r="VM3" s="0"/>
-      <c r="VN3" s="0"/>
-      <c r="VO3" s="0"/>
-      <c r="VP3" s="0"/>
-      <c r="VQ3" s="0"/>
-      <c r="VR3" s="0"/>
-      <c r="VS3" s="0"/>
-      <c r="VT3" s="0"/>
-      <c r="VU3" s="0"/>
-      <c r="VV3" s="0"/>
-      <c r="VW3" s="0"/>
-      <c r="VX3" s="0"/>
-      <c r="VY3" s="0"/>
-      <c r="VZ3" s="0"/>
-      <c r="WA3" s="0"/>
-      <c r="WB3" s="0"/>
-      <c r="WC3" s="0"/>
-      <c r="WD3" s="0"/>
-      <c r="WE3" s="0"/>
-      <c r="WF3" s="0"/>
-      <c r="WG3" s="0"/>
-      <c r="WH3" s="0"/>
-      <c r="WI3" s="0"/>
-      <c r="WJ3" s="0"/>
-      <c r="WK3" s="0"/>
-      <c r="WL3" s="0"/>
-      <c r="WM3" s="0"/>
-      <c r="WN3" s="0"/>
-      <c r="WO3" s="0"/>
-      <c r="WP3" s="0"/>
-      <c r="WQ3" s="0"/>
-      <c r="WR3" s="0"/>
-      <c r="WS3" s="0"/>
-      <c r="WT3" s="0"/>
-      <c r="WU3" s="0"/>
-      <c r="WV3" s="0"/>
-      <c r="WW3" s="0"/>
-      <c r="WX3" s="0"/>
-      <c r="WY3" s="0"/>
-      <c r="WZ3" s="0"/>
-      <c r="XA3" s="0"/>
-      <c r="XB3" s="0"/>
-      <c r="XC3" s="0"/>
-      <c r="XD3" s="0"/>
-      <c r="XE3" s="0"/>
-      <c r="XF3" s="0"/>
-      <c r="XG3" s="0"/>
-      <c r="XH3" s="0"/>
-      <c r="XI3" s="0"/>
-      <c r="XJ3" s="0"/>
-      <c r="XK3" s="0"/>
-      <c r="XL3" s="0"/>
-      <c r="XM3" s="0"/>
-      <c r="XN3" s="0"/>
-      <c r="XO3" s="0"/>
-      <c r="XP3" s="0"/>
-      <c r="XQ3" s="0"/>
-      <c r="XR3" s="0"/>
-      <c r="XS3" s="0"/>
-      <c r="XT3" s="0"/>
-      <c r="XU3" s="0"/>
-      <c r="XV3" s="0"/>
-      <c r="XW3" s="0"/>
-      <c r="XX3" s="0"/>
-      <c r="XY3" s="0"/>
-      <c r="XZ3" s="0"/>
-      <c r="YA3" s="0"/>
-      <c r="YB3" s="0"/>
-      <c r="YC3" s="0"/>
-      <c r="YD3" s="0"/>
-      <c r="YE3" s="0"/>
-      <c r="YF3" s="0"/>
-      <c r="YG3" s="0"/>
-      <c r="YH3" s="0"/>
-      <c r="YI3" s="0"/>
-      <c r="YJ3" s="0"/>
-      <c r="YK3" s="0"/>
-      <c r="YL3" s="0"/>
-      <c r="YM3" s="0"/>
-      <c r="YN3" s="0"/>
-      <c r="YO3" s="0"/>
-      <c r="YP3" s="0"/>
-      <c r="YQ3" s="0"/>
-      <c r="YR3" s="0"/>
-      <c r="YS3" s="0"/>
-      <c r="YT3" s="0"/>
-      <c r="YU3" s="0"/>
-      <c r="YV3" s="0"/>
-      <c r="YW3" s="0"/>
-      <c r="YX3" s="0"/>
-      <c r="YY3" s="0"/>
-      <c r="YZ3" s="0"/>
-      <c r="ZA3" s="0"/>
-      <c r="ZB3" s="0"/>
-      <c r="ZC3" s="0"/>
-      <c r="ZD3" s="0"/>
-      <c r="ZE3" s="0"/>
-      <c r="ZF3" s="0"/>
-      <c r="ZG3" s="0"/>
-      <c r="ZH3" s="0"/>
-      <c r="ZI3" s="0"/>
-      <c r="ZJ3" s="0"/>
-      <c r="ZK3" s="0"/>
-      <c r="ZL3" s="0"/>
-      <c r="ZM3" s="0"/>
-      <c r="ZN3" s="0"/>
-      <c r="ZO3" s="0"/>
-      <c r="ZP3" s="0"/>
-      <c r="ZQ3" s="0"/>
-      <c r="ZR3" s="0"/>
-      <c r="ZS3" s="0"/>
-      <c r="ZT3" s="0"/>
-      <c r="ZU3" s="0"/>
-      <c r="ZV3" s="0"/>
-      <c r="ZW3" s="0"/>
-      <c r="ZX3" s="0"/>
-      <c r="ZY3" s="0"/>
-      <c r="ZZ3" s="0"/>
-      <c r="AAA3" s="0"/>
-      <c r="AAB3" s="0"/>
-      <c r="AAC3" s="0"/>
-      <c r="AAD3" s="0"/>
-      <c r="AAE3" s="0"/>
-      <c r="AAF3" s="0"/>
-      <c r="AAG3" s="0"/>
-      <c r="AAH3" s="0"/>
-      <c r="AAI3" s="0"/>
-      <c r="AAJ3" s="0"/>
-      <c r="AAK3" s="0"/>
-      <c r="AAL3" s="0"/>
-      <c r="AAM3" s="0"/>
-      <c r="AAN3" s="0"/>
-      <c r="AAO3" s="0"/>
-      <c r="AAP3" s="0"/>
-      <c r="AAQ3" s="0"/>
-      <c r="AAR3" s="0"/>
-      <c r="AAS3" s="0"/>
-      <c r="AAT3" s="0"/>
-      <c r="AAU3" s="0"/>
-      <c r="AAV3" s="0"/>
-      <c r="AAW3" s="0"/>
-      <c r="AAX3" s="0"/>
-      <c r="AAY3" s="0"/>
-      <c r="AAZ3" s="0"/>
-      <c r="ABA3" s="0"/>
-      <c r="ABB3" s="0"/>
-      <c r="ABC3" s="0"/>
-      <c r="ABD3" s="0"/>
-      <c r="ABE3" s="0"/>
-      <c r="ABF3" s="0"/>
-      <c r="ABG3" s="0"/>
-      <c r="ABH3" s="0"/>
-      <c r="ABI3" s="0"/>
-      <c r="ABJ3" s="0"/>
-      <c r="ABK3" s="0"/>
-      <c r="ABL3" s="0"/>
-      <c r="ABM3" s="0"/>
-      <c r="ABN3" s="0"/>
-      <c r="ABO3" s="0"/>
-      <c r="ABP3" s="0"/>
-      <c r="ABQ3" s="0"/>
-      <c r="ABR3" s="0"/>
-      <c r="ABS3" s="0"/>
-      <c r="ABT3" s="0"/>
-      <c r="ABU3" s="0"/>
-      <c r="ABV3" s="0"/>
-      <c r="ABW3" s="0"/>
-      <c r="ABX3" s="0"/>
-      <c r="ABY3" s="0"/>
-      <c r="ABZ3" s="0"/>
-      <c r="ACA3" s="0"/>
-      <c r="ACB3" s="0"/>
-      <c r="ACC3" s="0"/>
-      <c r="ACD3" s="0"/>
-      <c r="ACE3" s="0"/>
-      <c r="ACF3" s="0"/>
-      <c r="ACG3" s="0"/>
-      <c r="ACH3" s="0"/>
-      <c r="ACI3" s="0"/>
-      <c r="ACJ3" s="0"/>
-      <c r="ACK3" s="0"/>
-      <c r="ACL3" s="0"/>
-      <c r="ACM3" s="0"/>
-      <c r="ACN3" s="0"/>
-      <c r="ACO3" s="0"/>
-      <c r="ACP3" s="0"/>
-      <c r="ACQ3" s="0"/>
-      <c r="ACR3" s="0"/>
-      <c r="ACS3" s="0"/>
-      <c r="ACT3" s="0"/>
-      <c r="ACU3" s="0"/>
-      <c r="ACV3" s="0"/>
-      <c r="ACW3" s="0"/>
-      <c r="ACX3" s="0"/>
-      <c r="ACY3" s="0"/>
-      <c r="ACZ3" s="0"/>
-      <c r="ADA3" s="0"/>
-      <c r="ADB3" s="0"/>
-      <c r="ADC3" s="0"/>
-      <c r="ADD3" s="0"/>
-      <c r="ADE3" s="0"/>
-      <c r="ADF3" s="0"/>
-      <c r="ADG3" s="0"/>
-      <c r="ADH3" s="0"/>
-      <c r="ADI3" s="0"/>
-      <c r="ADJ3" s="0"/>
-      <c r="ADK3" s="0"/>
-      <c r="ADL3" s="0"/>
-      <c r="ADM3" s="0"/>
-      <c r="ADN3" s="0"/>
-      <c r="ADO3" s="0"/>
-      <c r="ADP3" s="0"/>
-      <c r="ADQ3" s="0"/>
-      <c r="ADR3" s="0"/>
-      <c r="ADS3" s="0"/>
-      <c r="ADT3" s="0"/>
-      <c r="ADU3" s="0"/>
-      <c r="ADV3" s="0"/>
-      <c r="ADW3" s="0"/>
-      <c r="ADX3" s="0"/>
-      <c r="ADY3" s="0"/>
-      <c r="ADZ3" s="0"/>
-      <c r="AEA3" s="0"/>
-      <c r="AEB3" s="0"/>
-      <c r="AEC3" s="0"/>
-      <c r="AED3" s="0"/>
-      <c r="AEE3" s="0"/>
-      <c r="AEF3" s="0"/>
-      <c r="AEG3" s="0"/>
-      <c r="AEH3" s="0"/>
-      <c r="AEI3" s="0"/>
-      <c r="AEJ3" s="0"/>
-      <c r="AEK3" s="0"/>
-      <c r="AEL3" s="0"/>
-      <c r="AEM3" s="0"/>
-      <c r="AEN3" s="0"/>
-      <c r="AEO3" s="0"/>
-      <c r="AEP3" s="0"/>
-      <c r="AEQ3" s="0"/>
-      <c r="AER3" s="0"/>
-      <c r="AES3" s="0"/>
-      <c r="AET3" s="0"/>
-      <c r="AEU3" s="0"/>
-      <c r="AEV3" s="0"/>
-      <c r="AEW3" s="0"/>
-      <c r="AEX3" s="0"/>
-      <c r="AEY3" s="0"/>
-      <c r="AEZ3" s="0"/>
-      <c r="AFA3" s="0"/>
-      <c r="AFB3" s="0"/>
-      <c r="AFC3" s="0"/>
-      <c r="AFD3" s="0"/>
-      <c r="AFE3" s="0"/>
-      <c r="AFF3" s="0"/>
-      <c r="AFG3" s="0"/>
-      <c r="AFH3" s="0"/>
-      <c r="AFI3" s="0"/>
-      <c r="AFJ3" s="0"/>
-      <c r="AFK3" s="0"/>
-      <c r="AFL3" s="0"/>
-      <c r="AFM3" s="0"/>
-      <c r="AFN3" s="0"/>
-      <c r="AFO3" s="0"/>
-      <c r="AFP3" s="0"/>
-      <c r="AFQ3" s="0"/>
-      <c r="AFR3" s="0"/>
-      <c r="AFS3" s="0"/>
-      <c r="AFT3" s="0"/>
-      <c r="AFU3" s="0"/>
-      <c r="AFV3" s="0"/>
-      <c r="AFW3" s="0"/>
-      <c r="AFX3" s="0"/>
-      <c r="AFY3" s="0"/>
-      <c r="AFZ3" s="0"/>
-      <c r="AGA3" s="0"/>
-      <c r="AGB3" s="0"/>
-      <c r="AGC3" s="0"/>
-      <c r="AGD3" s="0"/>
-      <c r="AGE3" s="0"/>
-      <c r="AGF3" s="0"/>
-      <c r="AGG3" s="0"/>
-      <c r="AGH3" s="0"/>
-      <c r="AGI3" s="0"/>
-      <c r="AGJ3" s="0"/>
-      <c r="AGK3" s="0"/>
-      <c r="AGL3" s="0"/>
-      <c r="AGM3" s="0"/>
-      <c r="AGN3" s="0"/>
-      <c r="AGO3" s="0"/>
-      <c r="AGP3" s="0"/>
-      <c r="AGQ3" s="0"/>
-      <c r="AGR3" s="0"/>
-      <c r="AGS3" s="0"/>
-      <c r="AGT3" s="0"/>
-      <c r="AGU3" s="0"/>
-      <c r="AGV3" s="0"/>
-      <c r="AGW3" s="0"/>
-      <c r="AGX3" s="0"/>
-      <c r="AGY3" s="0"/>
-      <c r="AGZ3" s="0"/>
-      <c r="AHA3" s="0"/>
-      <c r="AHB3" s="0"/>
-      <c r="AHC3" s="0"/>
-      <c r="AHD3" s="0"/>
-      <c r="AHE3" s="0"/>
-      <c r="AHF3" s="0"/>
-      <c r="AHG3" s="0"/>
-      <c r="AHH3" s="0"/>
-      <c r="AHI3" s="0"/>
-      <c r="AHJ3" s="0"/>
-      <c r="AHK3" s="0"/>
-      <c r="AHL3" s="0"/>
-      <c r="AHM3" s="0"/>
-      <c r="AHN3" s="0"/>
-      <c r="AHO3" s="0"/>
-      <c r="AHP3" s="0"/>
-      <c r="AHQ3" s="0"/>
-      <c r="AHR3" s="0"/>
-      <c r="AHS3" s="0"/>
-      <c r="AHT3" s="0"/>
-      <c r="AHU3" s="0"/>
-      <c r="AHV3" s="0"/>
-      <c r="AHW3" s="0"/>
-      <c r="AHX3" s="0"/>
-      <c r="AHY3" s="0"/>
-      <c r="AHZ3" s="0"/>
-      <c r="AIA3" s="0"/>
-      <c r="AIB3" s="0"/>
-      <c r="AIC3" s="0"/>
-      <c r="AID3" s="0"/>
-      <c r="AIE3" s="0"/>
-      <c r="AIF3" s="0"/>
-      <c r="AIG3" s="0"/>
-      <c r="AIH3" s="0"/>
-      <c r="AII3" s="0"/>
-      <c r="AIJ3" s="0"/>
-      <c r="AIK3" s="0"/>
-      <c r="AIL3" s="0"/>
-      <c r="AIM3" s="0"/>
-      <c r="AIN3" s="0"/>
-      <c r="AIO3" s="0"/>
-      <c r="AIP3" s="0"/>
-      <c r="AIQ3" s="0"/>
-      <c r="AIR3" s="0"/>
-      <c r="AIS3" s="0"/>
-      <c r="AIT3" s="0"/>
-      <c r="AIU3" s="0"/>
-      <c r="AIV3" s="0"/>
-      <c r="AIW3" s="0"/>
-      <c r="AIX3" s="0"/>
-      <c r="AIY3" s="0"/>
-      <c r="AIZ3" s="0"/>
-      <c r="AJA3" s="0"/>
-      <c r="AJB3" s="0"/>
-      <c r="AJC3" s="0"/>
-      <c r="AJD3" s="0"/>
-      <c r="AJE3" s="0"/>
-      <c r="AJF3" s="0"/>
-      <c r="AJG3" s="0"/>
-      <c r="AJH3" s="0"/>
-      <c r="AJI3" s="0"/>
-      <c r="AJJ3" s="0"/>
-      <c r="AJK3" s="0"/>
-      <c r="AJL3" s="0"/>
-      <c r="AJM3" s="0"/>
-      <c r="AJN3" s="0"/>
-      <c r="AJO3" s="0"/>
-      <c r="AJP3" s="0"/>
-      <c r="AJQ3" s="0"/>
-      <c r="AJR3" s="0"/>
-      <c r="AJS3" s="0"/>
-      <c r="AJT3" s="0"/>
-      <c r="AJU3" s="0"/>
-      <c r="AJV3" s="0"/>
-      <c r="AJW3" s="0"/>
-      <c r="AJX3" s="0"/>
-      <c r="AJY3" s="0"/>
-      <c r="AJZ3" s="0"/>
-      <c r="AKA3" s="0"/>
-      <c r="AKB3" s="0"/>
-      <c r="AKC3" s="0"/>
-      <c r="AKD3" s="0"/>
-      <c r="AKE3" s="0"/>
-      <c r="AKF3" s="0"/>
-      <c r="AKG3" s="0"/>
-      <c r="AKH3" s="0"/>
-      <c r="AKI3" s="0"/>
-      <c r="AKJ3" s="0"/>
-      <c r="AKK3" s="0"/>
-      <c r="AKL3" s="0"/>
-      <c r="AKM3" s="0"/>
-      <c r="AKN3" s="0"/>
-      <c r="AKO3" s="0"/>
-      <c r="AKP3" s="0"/>
-      <c r="AKQ3" s="0"/>
-      <c r="AKR3" s="0"/>
-      <c r="AKS3" s="0"/>
-      <c r="AKT3" s="0"/>
-      <c r="AKU3" s="0"/>
-      <c r="AKV3" s="0"/>
-      <c r="AKW3" s="0"/>
-      <c r="AKX3" s="0"/>
-      <c r="AKY3" s="0"/>
-      <c r="AKZ3" s="0"/>
-      <c r="ALA3" s="0"/>
-      <c r="ALB3" s="0"/>
-      <c r="ALC3" s="0"/>
-      <c r="ALD3" s="0"/>
-      <c r="ALE3" s="0"/>
-      <c r="ALF3" s="0"/>
-      <c r="ALG3" s="0"/>
-      <c r="ALH3" s="0"/>
-      <c r="ALI3" s="0"/>
-      <c r="ALJ3" s="0"/>
-      <c r="ALK3" s="0"/>
-      <c r="ALL3" s="0"/>
-      <c r="ALM3" s="0"/>
-      <c r="ALN3" s="0"/>
-      <c r="ALO3" s="0"/>
-      <c r="ALP3" s="0"/>
-      <c r="ALQ3" s="0"/>
-      <c r="ALR3" s="0"/>
-      <c r="ALS3" s="0"/>
-      <c r="ALT3" s="0"/>
-      <c r="ALU3" s="0"/>
-      <c r="ALV3" s="0"/>
-      <c r="ALW3" s="0"/>
-      <c r="ALX3" s="0"/>
-      <c r="ALY3" s="0"/>
-      <c r="ALZ3" s="0"/>
-      <c r="AMA3" s="0"/>
-      <c r="AMB3" s="0"/>
-      <c r="AMC3" s="0"/>
-      <c r="AMD3" s="0"/>
-      <c r="AME3" s="0"/>
-      <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>19</v>
@@ -3306,34 +2266,34 @@
       <c r="T5" s="0"/>
       <c r="U5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>19</v>
@@ -3349,34 +2309,34 @@
       <c r="T6" s="0"/>
       <c r="U6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>19</v>
@@ -3392,34 +2352,34 @@
       <c r="T7" s="0"/>
       <c r="U7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="7"/>
+      <c r="F8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>19</v>
@@ -3435,34 +2395,34 @@
       <c r="T8" s="0"/>
       <c r="U8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>19</v>
@@ -3478,34 +2438,34 @@
       <c r="T9" s="0"/>
       <c r="U9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="7"/>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>19</v>
@@ -3521,34 +2481,34 @@
       <c r="T10" s="0"/>
       <c r="U10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
+    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>330</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="7" t="n">
-        <v>11</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="I11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>19</v>
@@ -3564,33 +2524,33 @@
       <c r="T11" s="0"/>
       <c r="U11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>330</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="5" t="s">
         <v>55</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -3608,37 +2568,17 @@
       <c r="U12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -3651,17 +2591,39 @@
       <c r="U13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>1206</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
       <c r="N14" s="0"/>
@@ -3674,35 +2636,35 @@
       <c r="U14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="6" t="n">
-        <v>1206</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>66</v>
+      <c r="J15" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>19</v>
@@ -3719,35 +2681,35 @@
       <c r="U15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>68</v>
       </c>
+      <c r="B16" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="6" t="n">
-        <v>1206</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>70</v>
+      <c r="J16" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>19</v>
@@ -3764,35 +2726,35 @@
       <c r="U16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>72</v>
+      <c r="A17" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="6" t="n">
-        <v>1210</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>75</v>
+      <c r="J17" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>19</v>
@@ -3809,35 +2771,35 @@
       <c r="U17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>77</v>
+      <c r="A18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>79</v>
+      <c r="G18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>19</v>
@@ -3854,35 +2816,35 @@
       <c r="U18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>81</v>
+      <c r="A19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>85</v>
+      <c r="J19" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>19</v>
@@ -3899,35 +2861,35 @@
       <c r="U19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>87</v>
+      <c r="A20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I20" s="6" t="s">
+      <c r="G20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>89</v>
+      <c r="J20" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>19</v>
@@ -3944,39 +2906,16 @@
       <c r="U20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="7" t="n">
-        <v>15</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
       <c r="N21" s="0"/>
@@ -3989,39 +2928,34 @@
       <c r="U21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="I22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J22" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="K22" s="7"/>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
@@ -4034,39 +2968,34 @@
       <c r="U22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="G23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="6" t="s">
+      <c r="I23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="K23" s="7"/>
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
@@ -4079,16 +3008,34 @@
       <c r="U23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+      <c r="A24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K24" s="7"/>
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -4100,35 +3047,37 @@
       <c r="T24" s="0"/>
       <c r="U24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="7" t="n">
+    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H25" s="6" t="s">
+      <c r="C25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="6" t="s">
+      <c r="F25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="K25" s="5"/>
+      <c r="H25" s="9" t="n">
+        <v>744786131</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -4141,34 +3090,16 @@
       <c r="U25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="K26" s="5"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="7"/>
       <c r="L26" s="0"/>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -4181,34 +3112,36 @@
       <c r="U26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="I27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="K27" s="5"/>
+      <c r="K27" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L27" s="0"/>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -4220,300 +3153,290 @@
       <c r="T27" s="0"/>
       <c r="U27" s="0"/>
     </row>
-    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H28" s="9" t="n">
-        <v>744786131</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J28" s="6" t="s">
+      <c r="I28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>123</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="0"/>
-      <c r="M28" s="0"/>
-      <c r="N28" s="0"/>
-      <c r="O28" s="0"/>
-      <c r="P28" s="0"/>
-      <c r="Q28" s="0"/>
-      <c r="R28" s="0"/>
-      <c r="S28" s="0"/>
-      <c r="T28" s="0"/>
-      <c r="U28" s="0"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="0"/>
-      <c r="M29" s="0"/>
-      <c r="N29" s="0"/>
-      <c r="O29" s="0"/>
-      <c r="P29" s="0"/>
-      <c r="Q29" s="0"/>
-      <c r="R29" s="0"/>
-      <c r="S29" s="0"/>
-      <c r="T29" s="0"/>
-      <c r="U29" s="0"/>
+      <c r="A29" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="7" t="n">
+      <c r="A30" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="6" t="s">
+      <c r="C30" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J30" s="6" t="s">
-        <v>130</v>
+      <c r="J30" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L30" s="0"/>
-      <c r="M30" s="0"/>
-      <c r="N30" s="0"/>
-      <c r="O30" s="0"/>
-      <c r="P30" s="0"/>
-      <c r="Q30" s="0"/>
-      <c r="R30" s="0"/>
-      <c r="S30" s="0"/>
-      <c r="T30" s="0"/>
-      <c r="U30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="2" t="n">
+      <c r="A31" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="I31" s="2" t="s">
+      <c r="C31" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
+      <c r="J31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="K31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B32" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="I32" s="6" t="s">
+      <c r="D32" s="5"/>
+      <c r="F32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="J32" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K32" s="7"/>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="H33" s="2" t="s">
+    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="B33" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>146</v>
+      <c r="J33" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="7" t="n">
+      <c r="A34" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="F34" s="6" t="s">
+      <c r="G34" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="I34" s="6" t="s">
+      <c r="H34" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="K34" s="5"/>
+      <c r="J34" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B35" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="A35" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="F35" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="I35" s="6" t="s">
+      <c r="G35" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="K35" s="5"/>
+      <c r="J35" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B36" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="F36" s="6" t="s">
+    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="B36" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="F36" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H36" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="I36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="9" t="s">
         <v>163</v>
       </c>
       <c r="K36" s="2" t="s">
@@ -4521,95 +3444,71 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="F38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B38" s="7" t="n">
+      <c r="I38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B39" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="I38" s="6" t="s">
+      <c r="C39" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="F39" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J38" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B39" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="9" t="s">
+      <c r="J39" s="5" t="s">
         <v>175</v>
       </c>
       <c r="K39" s="2" t="s">
@@ -4617,368 +3516,296 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
+      <c r="A40" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="F40" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B41" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="F41" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>182</v>
-      </c>
+      <c r="A41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="F42" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B42" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="G42" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="F42" s="6" t="s">
+      <c r="H42" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H42" s="6" t="s">
+      <c r="I42" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="I42" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="6" t="s">
+      <c r="J42" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B43" s="2" t="n">
+      <c r="B43" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="F43" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D43" s="5"/>
-      <c r="F43" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="H43" s="2" t="s">
+      <c r="G43" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="H43" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="I43" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K43" s="2" t="s">
+      <c r="J43" s="5" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
+      <c r="A44" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B44" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="F44" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="B45" s="7" t="n">
+      <c r="A45" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="F45" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="I45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="J45" s="6" t="s">
+      <c r="D45" s="5"/>
+      <c r="F45" s="5" t="s">
         <v>199</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B46" s="7" t="n">
+      <c r="A46" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="F46" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J46" s="6" t="s">
+      <c r="C46" s="5" t="s">
         <v>204</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="F46" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="B47" s="7" t="n">
+      <c r="A47" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B47" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="F47" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="I47" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>208</v>
+      <c r="C47" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="5"/>
+      <c r="F47" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B48" s="7" t="n">
+      <c r="A48" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B48" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="F48" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="I48" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>214</v>
+      </c>
+      <c r="D48" s="5"/>
+      <c r="F48" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="B49" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="F49" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J49" s="6" t="s">
+      <c r="A49" s="5" t="s">
         <v>219</v>
+      </c>
+      <c r="B49" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="F49" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="F50" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="I50" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>224</v>
-      </c>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B51" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="B51" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C51" s="6" t="s">
+      <c r="D51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="F51" s="6" t="s">
+      <c r="H51" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="G51" s="6" t="s">
+      <c r="I51" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J51" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="I51" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="J51" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="B52" s="7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="F52" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="I52" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J52" s="6" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="B54" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -5000,20 +3827,20 @@
   <dimension ref="1:18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.4534412955466"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="9.10526315789474"/>
   </cols>
@@ -5029,7 +3856,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -5050,7 +3877,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6080,29 +4907,29 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="B3" s="7" t="n">
+      <c r="A3" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="0"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>247</v>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -7134,17 +5961,17 @@
     </row>
     <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="2"/>
@@ -7152,26 +5979,26 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="K6" s="2" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="N6" s="0"/>
       <c r="O6" s="0"/>
@@ -8187,21 +7014,21 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="K7" s="2" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="N7" s="0"/>
       <c r="O7" s="0"/>
@@ -9217,19 +8044,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="K8" s="2" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="N8" s="0"/>
       <c r="O8" s="0"/>
@@ -10245,21 +9072,21 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="K9" s="2" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="N9" s="0"/>
       <c r="O9" s="0"/>
@@ -11275,157 +10102,157 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="K10" s="2" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="K11" s="2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="K12" s="2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="K13" s="2" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="K14" s="2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
       <c r="K15" s="2" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
       <c r="K16" s="2" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="K17" s="2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
       <c r="K18" s="2" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -11462,11 +10289,11 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="5.78542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="9.10526315789474"/>
   </cols>
@@ -11503,104 +10330,104 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="B3" s="7" t="n">
+      <c r="A3" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>288</v>
+      <c r="D3" s="5" t="s">
+        <v>276</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="F3" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="G3" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="K3" s="6"/>
+      <c r="J3" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="13"/>
     </row>
     <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="B5" s="7" t="n">
+      <c r="A5" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>102</v>
+      <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="F5" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="G5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K5" s="6"/>
+      <c r="J5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E6" s="13"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="B7" s="7" t="n">
+      <c r="A7" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="D7" s="6"/>
+      <c r="C7" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+        <v>277</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
@@ -11617,17 +10444,17 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="0"/>
@@ -11651,16 +10478,17 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>299</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="D11" s="0"/>
       <c r="E11" s="13" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="1"/>
@@ -11668,26 +10496,26 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="F12" s="13"/>
       <c r="K12" s="2" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated documentation and other small changes
</commit_message>
<xml_diff>
--- a/Doc/BOM.xlsx
+++ b/Doc/BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="285">
   <si>
     <t xml:space="preserve">Ref.Des.</t>
   </si>
@@ -57,13 +57,13 @@
     <t xml:space="preserve">notes</t>
   </si>
   <si>
-    <t xml:space="preserve">R7</t>
+    <t xml:space="preserve">R2, R3, R4, R5, R7, R10, R21, R40, R41, R43, R44, R45, R46, R52, R53, R54</t>
   </si>
   <si>
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
-    <t xml:space="preserve">2k4</t>
+    <t xml:space="preserve">1k8</t>
   </si>
   <si>
     <t xml:space="preserve">0603</t>
@@ -72,19 +72,19 @@
     <t xml:space="preserve">Yageo</t>
   </si>
   <si>
-    <t xml:space="preserve">RC0603JR-072K4L</t>
+    <t xml:space="preserve">RC0603FR-071K8L</t>
   </si>
   <si>
     <t xml:space="preserve">Mouser</t>
   </si>
   <si>
-    <t xml:space="preserve">603-RC0603JR-072K4L</t>
+    <t xml:space="preserve">603-RC0603FR-071K8L</t>
   </si>
   <si>
     <t xml:space="preserve">exact part my be changed</t>
   </si>
   <si>
-    <t xml:space="preserve">R22</t>
+    <t xml:space="preserve">R23</t>
   </si>
   <si>
     <t xml:space="preserve">82k</t>
@@ -96,7 +96,7 @@
     <t xml:space="preserve">603-RC0603FR-0782KL</t>
   </si>
   <si>
-    <t xml:space="preserve">R1, R11, R23</t>
+    <t xml:space="preserve">R1, R11, R24</t>
   </si>
   <si>
     <t xml:space="preserve">180k</t>
@@ -108,19 +108,7 @@
     <t xml:space="preserve">603-RC0603JR-07180KL</t>
   </si>
   <si>
-    <t xml:space="preserve">R30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-0747KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-0747KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R6, R10, R21</t>
+    <t xml:space="preserve">R6, R22</t>
   </si>
   <si>
     <t xml:space="preserve">12k</t>
@@ -132,7 +120,7 @@
     <t xml:space="preserve">603-RC0603FR-0712KL</t>
   </si>
   <si>
-    <t xml:space="preserve">R12, R24</t>
+    <t xml:space="preserve">R12, R25</t>
   </si>
   <si>
     <t xml:space="preserve">34k</t>
@@ -144,31 +132,7 @@
     <t xml:space="preserve">603-RC0603FR-0734KL</t>
   </si>
   <si>
-    <t xml:space="preserve">R33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5k1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-075K1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-075K1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2,R3,R4,R5,R32,R40,R41,R43,R44,R45,R46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1k6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0603FR-071K6L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">603-RC0603FR-071K6L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R47,R48,R49,R50,R51</t>
+    <t xml:space="preserve">R47, R48, R49, R50, R51</t>
   </si>
   <si>
     <t xml:space="preserve">RC0603FR-07330RL</t>
@@ -177,28 +141,13 @@
     <t xml:space="preserve">603-RC0603FR-07330RL</t>
   </si>
   <si>
-    <t xml:space="preserve">R31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0R1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panasonic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERJ-3RSFR10V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">667-ERJ-3RSFR10V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C16, C24</t>
+    <t xml:space="preserve">C16, C26</t>
   </si>
   <si>
     <t xml:space="preserve">Capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">100µF</t>
+    <t xml:space="preserve">100µ</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;5V</t>
@@ -213,10 +162,10 @@
     <t xml:space="preserve">81-GRM31CR60J107ME9L</t>
   </si>
   <si>
-    <t xml:space="preserve">C10, C11, C12, C20, C30, C34, C52, C54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10µF</t>
+    <t xml:space="preserve">C10, C11, C12, C20, C21, C30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10µ</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;24V</t>
@@ -228,7 +177,7 @@
     <t xml:space="preserve">81-GRM188R6YA106MA3D</t>
   </si>
   <si>
-    <t xml:space="preserve">C47,C48,C49</t>
+    <t xml:space="preserve">C40, C47, C48</t>
   </si>
   <si>
     <t xml:space="preserve">2µ2</t>
@@ -246,10 +195,10 @@
     <t xml:space="preserve">810-C1608X5R1V225K</t>
   </si>
   <si>
-    <t xml:space="preserve">C14, C15,C40,C51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1µF</t>
+    <t xml:space="preserve">C14, C15, C51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1µ</t>
   </si>
   <si>
     <t xml:space="preserve">GRM188R61E105KA12D</t>
@@ -258,13 +207,10 @@
     <t xml:space="preserve">81-GRM188R61E105KA12</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2,C13,C23,C32,C33,C41,C42,C43,C44, C50,C53,C55,C61,C62,C63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;10V</t>
+    <t xml:space="preserve">C1, C2, C3, C13, C22, C25, C31, C32, C41, C42, C43, C44, C49, C50, C53, C55, C61, C62, C63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100n</t>
   </si>
   <si>
     <t xml:space="preserve">Kemet</t>
@@ -279,10 +225,10 @@
     <t xml:space="preserve">801-5347</t>
   </si>
   <si>
-    <t xml:space="preserve">C21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.4nF</t>
+    <t xml:space="preserve">C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2n4</t>
   </si>
   <si>
     <t xml:space="preserve">GRM1885C1H242JA01D</t>
@@ -291,582 +237,624 @@
     <t xml:space="preserve">815-1474</t>
   </si>
   <si>
-    <t xml:space="preserve">C22</t>
+    <t xml:space="preserve">C24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM0335C1E220JA01D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-GRM0335C1E220JA1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33, C34, C52, C54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22µ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM188R60J226ME15D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-GRM188R60J226ME5D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL60XX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coilcraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL6030-222MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">994-XAL6030-222MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4µ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL4030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL4030-472MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">994-XAL4030-472MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bourns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRN4018TA-4R7M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-SRN4018TA-4R7M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS160808-1R0K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-CS160808-1R0K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1, FB2, FB3, FB4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferrite Bead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLM31KN471SN1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-BLM31KN471SN1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z-Diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD323-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM3Z18VST1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-MM3Z18VST1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD323F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM3Z24VB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-MM3Z24VB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3,D44,D45,D46,D47,D48,D49,D50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3V6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairchild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDZ3V6ASF-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-DDZ3V6ASF-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD-123-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nexperia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NZH5V1B,115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">771-NZH5V1B-115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schottky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO-221AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSSAF5M10HM3/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78-VSSAF5M10HM3/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD-123-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS24FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-SS24FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D40,D51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP2012EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-AP2012EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT2012YC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-APT2012YC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT2012SGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-APT2012SGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT2012QBC/D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-APT2012QBC/D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PowerPAK1212-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SISS27DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78-SISS27DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alternative: SISS27ADN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPN-Transistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC846BLT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-BC846BLT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIS488DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78-SIS488DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">better: SIS862DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switching regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFN14 4x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richtek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT7259GQW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1028-1199-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSOP-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Instruments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS54340DDAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-TPS54340DDAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QFN-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semtech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS30041-M033QFNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">947-TS30041-M033QFNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQFP-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32F401VBT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-STM32F401VBT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2xOR-Gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSSOP-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74LVC2G32DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">816-8820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M74VHC1G126DTT1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">805-1494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QFN-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invensense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICM-20689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1428-1059-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U44,U45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motordriver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSON-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRV8835DSSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">813-6485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pushbutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSM2JSMASTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">131-4776</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combined (preffered)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS-PRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPEG158-P5H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">771-6910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket 2x20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bottom Side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RaspberryPi3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket 1x4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART_EXT_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket 2x4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C_EXT_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C_EXT_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket 1x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket 3x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPI_EXT_0_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPI_EXT_0_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPI_EXT_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket 1x8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O_0-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O_8-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Socket 2x8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O_0-7 Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O_8-15 Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin 1x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin 3x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVO Signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pin 2x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVO Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J54, J55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOTORS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCT06030C2209FP500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">594-MCT06030C2209FP5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C45,C46</t>
   </si>
   <si>
     <t xml:space="preserve">22pF</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM0335C1E220JA01D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81-GRM0335C1E220JA1D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coilcraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL6030-222MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">994-XAL6030-222MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4µ7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL4030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL4030-472MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">994-XAL4030-472MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bourns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDR0403-4R7ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">736-1239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39nH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Würth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">883-0418</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-Diode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD323-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ON Semiconductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MM3Z18VST1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">863-MM3Z18VST1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD323F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MM3Z24VB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">512-MM3Z24VB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3,D44,D45,D46,D47,D48,D49,D50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3V6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fairchild</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDZ3V6ASF-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">621-DDZ3V6ASF-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5V2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD-123-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nexperia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NZH5V1B,115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">771-NZH5V1B-115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schottky</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> POWERDI-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diodes Incorporated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDS760-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">621-PDS760-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2, D30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD-123-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SS24FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">512-SS24FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D40,D51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kingbright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP2012EC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-AP2012EC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APT2012YC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-APT2012YC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APT2012SGC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-APT2012SGC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APT2012QBC/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-APT2012QBC/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-MOSFET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PowerPAK1212-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SISS27DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78-SISS27DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">better:: SISS27ADN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPN-Transistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BC846BLT3G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">863-BC846BLT3G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-MOSFET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIS434DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">781-SIS434DN-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">better: SIS862DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switching regulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DFN14 4x3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richtek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT7259GQW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1028-1199-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSOP-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas Instruments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPS54340DDAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">595-TPS54340DDAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSOP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LM25011MY/NOPB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">761-4883</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microcontroller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LQFP-100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F401VBT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">511-STM32F401VBT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2xOR-Gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSSOP-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74LVC2G32DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">816-8820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buffer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSOP-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M74VHC1G126DTT1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">805-1494</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QFN-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invensense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICM-20689</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1428-1059-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U44,U45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motordriver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WSON-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRV8835DSSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">813-6485</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pushbutton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FSM2JSMASTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">131-4776</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combined (preffered)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS-PRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPEG158-P5H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">771-6910</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket 2x20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bottom Side</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RaspberryPi3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket 1x4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UART_EXT_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket 2x4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C_EXT_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C_EXT_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket 1x6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket 3x6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPI_EXT_0_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPI_EXT_0_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPI_EXT_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket 1x8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I/O_0-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I/O_8-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Socket 2x8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I/O_0-7 Power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I/O_8-15 Power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pin 1x6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pin 3x6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVO Signal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pin 2x6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVO Power</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J54, J55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOTORS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCT06030C2209FP500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">594-MCT06030C2209FP5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C45,C46</t>
-  </si>
-  <si>
     <t xml:space="preserve">Y40</t>
   </si>
   <si>
@@ -874,12 +862,6 @@
   </si>
   <si>
     <t xml:space="preserve">HC49-4H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pin 1x2</t>
   </si>
   <si>
     <t xml:space="preserve">J2</t>
@@ -905,7 +887,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -948,6 +930,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -992,7 +980,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1025,7 +1013,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1034,6 +1034,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1066,25 +1070,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:51"/>
+  <dimension ref="1:50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.3076923076923"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="71.0323886639676"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.8542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1134,6 +1138,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
+      <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
@@ -2153,7 +2158,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>12</v>
@@ -2167,7 +2172,7 @@
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -2206,7 +2211,7 @@
       <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -2243,13 +2248,13 @@
       <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="9" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -2271,7 +2276,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
@@ -2286,13 +2291,13 @@
       <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="9" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="9" t="s">
         <v>31</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -2314,7 +2319,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -2329,13 +2334,13 @@
       <c r="G7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>34</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="9" t="s">
         <v>35</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -2357,13 +2362,13 @@
         <v>36</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>37</v>
+      <c r="D8" s="5" t="n">
+        <v>330</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="5" t="s">
@@ -2373,13 +2378,13 @@
         <v>15</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>39</v>
+      <c r="J8" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>19</v>
@@ -2395,38 +2400,18 @@
       <c r="T8" s="0"/>
       <c r="U8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>41</v>
-      </c>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
       <c r="N9" s="0"/>
@@ -2438,34 +2423,36 @@
       <c r="T9" s="0"/>
       <c r="U9" s="0"/>
     </row>
-    <row r="10" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>1206</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>47</v>
+      <c r="J10" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>19</v>
@@ -2481,25 +2468,27 @@
       <c r="T10" s="0"/>
       <c r="U10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>330</v>
-      </c>
-      <c r="E11" s="7"/>
       <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>49</v>
@@ -2507,7 +2496,7 @@
       <c r="I11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="8" t="s">
+      <c r="J11" s="5" t="s">
         <v>50</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -2529,29 +2518,31 @@
         <v>51</v>
       </c>
       <c r="B12" s="6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>19</v>
@@ -2568,17 +2559,39 @@
       <c r="U12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="A13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
@@ -2592,34 +2605,34 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B14" s="6" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>1206</v>
+        <v>48</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>19</v>
@@ -2637,34 +2650,34 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B15" s="6" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>19</v>
@@ -2682,34 +2695,34 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B16" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>19</v>
@@ -2727,34 +2740,34 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>4</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>76</v>
+        <v>43</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>19</v>
@@ -2771,39 +2784,16 @@
       <c r="U17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
@@ -2817,38 +2807,33 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="K19" s="7"/>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
       <c r="N19" s="0"/>
@@ -2862,38 +2847,33 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="K20" s="7"/>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
       <c r="N20" s="0"/>
@@ -2906,15 +2886,33 @@
       <c r="U20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="A21" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>94</v>
+      </c>
       <c r="K21" s="7"/>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
@@ -2927,35 +2925,37 @@
       <c r="T21" s="0"/>
       <c r="U21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>95</v>
+        <v>14</v>
       </c>
       <c r="G22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K22" s="7"/>
+        <v>97</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
@@ -2968,34 +2968,15 @@
       <c r="U22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="K23" s="7"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
@@ -3007,35 +2988,40 @@
       <c r="T23" s="0"/>
       <c r="U23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B24" s="6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>100</v>
       </c>
+      <c r="E24" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="F24" s="5" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>106</v>
+        <v>43</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="K24" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -3047,37 +3033,17 @@
       <c r="T24" s="0"/>
       <c r="U24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B25" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H25" s="9" t="n">
-        <v>744786131</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="7"/>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -3090,16 +3056,36 @@
       <c r="U25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="7"/>
+      <c r="A26" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L26" s="0"/>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -3112,147 +3098,137 @@
       <c r="U26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="6" t="n">
+      <c r="B27" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="I27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="0"/>
-      <c r="M27" s="0"/>
-      <c r="N27" s="0"/>
-      <c r="O27" s="0"/>
-      <c r="P27" s="0"/>
-      <c r="Q27" s="0"/>
-      <c r="R27" s="0"/>
-      <c r="S27" s="0"/>
-      <c r="T27" s="0"/>
-      <c r="U27" s="0"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="H28" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="I28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="G29" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G29" s="5" t="s">
+      <c r="H29" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="I29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="5" t="s">
         <v>134</v>
       </c>
       <c r="K30" s="2" t="s">
@@ -3267,81 +3243,89 @@
         <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D31" s="5"/>
       <c r="F31" s="5" t="s">
         <v>137</v>
       </c>
       <c r="G31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H31" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J31" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
         <v>140</v>
-      </c>
-      <c r="K31" s="7"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="B32" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D32" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="F32" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J32" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="K32" s="7"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>19</v>
@@ -3349,128 +3333,126 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="H34" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="I34" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="H35" s="12" t="s">
         <v>157</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>158</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="5" t="s">
-        <v>159</v>
+      <c r="J35" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B36" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
+      <c r="A37" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="F37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B38" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D38" s="5"/>
-      <c r="F38" s="2" t="s">
-        <v>166</v>
+      <c r="F38" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>168</v>
@@ -3482,183 +3464,180 @@
         <v>169</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>170</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B39" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="D39" s="7"/>
+      <c r="F39" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H39" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="D39" s="5"/>
-      <c r="F39" s="5" t="s">
+      <c r="I39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H39" s="5" t="s">
+      <c r="K39" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B40" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D40" s="7"/>
-      <c r="F40" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
+      <c r="A41" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B41" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="D41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
+      <c r="F41" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B42" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="5" t="s">
         <v>183</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="H42" s="5" t="s">
         <v>185</v>
       </c>
       <c r="I42" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B43" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D43" s="5"/>
       <c r="F43" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="H43" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>191</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B44" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="D44" s="5"/>
       <c r="F44" s="5" t="s">
         <v>194</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B45" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D45" s="5"/>
       <c r="F45" s="5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>201</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="J45" s="5" t="s">
         <v>202</v>
@@ -3675,17 +3654,17 @@
         <v>204</v>
       </c>
       <c r="D46" s="5"/>
-      <c r="F46" s="5" t="s">
+      <c r="F46" s="10" t="s">
         <v>205</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>206</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="J46" s="5" t="s">
         <v>207</v>
@@ -3706,106 +3685,82 @@
         <v>210</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>116</v>
+        <v>211</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B48" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D48" s="5"/>
       <c r="F48" s="5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>217</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>186</v>
+        <v>65</v>
       </c>
       <c r="J48" s="5" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B49" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="F49" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B51" s="6" t="n">
+      <c r="A50" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B50" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="D51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>228</v>
+      <c r="C50" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K50" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -3827,20 +3782,20 @@
   <dimension ref="1:18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="9.10526315789474"/>
   </cols>
@@ -3856,7 +3811,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -3877,7 +3832,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4908,28 +4863,28 @@
     </row>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="0"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -5961,17 +5916,17 @@
     </row>
     <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="2"/>
@@ -5979,26 +5934,26 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="K6" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="N6" s="0"/>
       <c r="O6" s="0"/>
@@ -7014,21 +6969,21 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>244</v>
+        <v>236</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>239</v>
       </c>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="K7" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="N7" s="0"/>
       <c r="O7" s="0"/>
@@ -8044,19 +7999,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D8" s="11"/>
+        <v>236</v>
+      </c>
+      <c r="D8" s="15"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="K8" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N8" s="0"/>
       <c r="O8" s="0"/>
@@ -9072,21 +9027,21 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>250</v>
+        <v>244</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>245</v>
       </c>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="K9" s="2" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="N9" s="0"/>
       <c r="O9" s="0"/>
@@ -10102,157 +10057,157 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D10" s="11"/>
+        <v>244</v>
+      </c>
+      <c r="D10" s="15"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="K10" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="D11" s="11"/>
+        <v>244</v>
+      </c>
+      <c r="D11" s="15"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="K11" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="K12" s="2" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="K13" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="K14" s="2" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
       <c r="K15" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>268</v>
+        <v>262</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>263</v>
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
       <c r="K16" s="2" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D17" s="11"/>
+        <v>266</v>
+      </c>
+      <c r="D17" s="15"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="K17" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
       <c r="K18" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -10276,10 +10231,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10291,9 +10246,9 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="9.10526315789474"/>
   </cols>
@@ -10330,13 +10285,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
-    <row r="2" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
@@ -10345,83 +10300,83 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>277</v>
+        <v>271</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="13"/>
+    <row r="4" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="17"/>
     </row>
     <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="13"/>
+    <row r="6" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="17"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="13" t="s">
-        <v>277</v>
+      <c r="E7" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -10430,12 +10385,12 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
@@ -10444,78 +10399,44 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="0"/>
-      <c r="H9" s="0"/>
-      <c r="I9" s="0"/>
-      <c r="J9" s="0"/>
-      <c r="K9" s="0"/>
+        <v>281</v>
+      </c>
+      <c r="D9" s="0"/>
+      <c r="E9" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="2" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
-      <c r="J10" s="0"/>
-      <c r="K10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="B11" s="2" t="n">
+      <c r="A10" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="D11" s="0"/>
-      <c r="E11" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="K12" s="2" t="s">
-        <v>290</v>
+      <c r="C10" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="K10" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes for first production version v1.0: added bootstrap resistor R26 R54 Pullup 5V MS Zones bigger U10 Pin7 GND silk improvements version changed: silk, sch & pcb pages updated doc files
</commit_message>
<xml_diff>
--- a/Doc/BOM.xlsx
+++ b/Doc/BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="290">
   <si>
     <t xml:space="preserve">Ref.Des.</t>
   </si>
@@ -141,6 +141,18 @@
     <t xml:space="preserve">603-RC0603FR-07330RL</t>
   </si>
   <si>
+    <t xml:space="preserve">R26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603JR-078R2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">603-RC0603JR-078R2L</t>
+  </si>
+  <si>
     <t xml:space="preserve">C16, C26</t>
   </si>
   <si>
@@ -201,10 +213,16 @@
     <t xml:space="preserve">1µ</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM188R61E105KA12D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81-GRM188R61E105KA12</t>
+    <t xml:space="preserve">&gt;6V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Würth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">885012106022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710-885012106022</t>
   </si>
   <si>
     <t xml:space="preserve">C1, C2, C3, C13, C22, C25, C31, C32, C41, C42, C43, C44, C49, C50, C53, C55, C61, C62, C63</t>
@@ -213,505 +231,502 @@
     <t xml:space="preserve">100n</t>
   </si>
   <si>
+    <t xml:space="preserve">885012206071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">710-885012206071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2n4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kemet</t>
   </si>
   <si>
-    <t xml:space="preserve">C0603C104K5RACTU</t>
+    <t xml:space="preserve">C0603C242J8HACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80-C0603C242J8HACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM0335C1E220JA01D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-GRM0335C1E220JA1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33, C34, C52, C54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22µ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM188R60J226ME15D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-GRM188R60J226ME5D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL60XX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coilcraft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL6030-222MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">994-XAL6030-222MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4µ7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL4030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XAL4030-472MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">994-XAL4030-472MEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bourns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRN4018TA-4R7M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-SRN4018TA-4R7M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CS160808-1R0K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-CS160808-1R0K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FB1, FB2, FB3, FB4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferrite Bead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLM31KN471SN1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81-BLM31KN471SN1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z-Diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD323-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON Semiconductor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM3Z18VST1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-MM3Z18VST1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD323F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM3Z24VB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-MM3Z24VB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3,D44,D45,D46,D47,D48,D49,D50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3V6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairchild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDZ3V6ASF-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">621-DDZ3V6ASF-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOD-123-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nexperia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NZH5V1B,115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">771-NZH5V1B-115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schottky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO-221AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSSAF5M10HM3/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78-VSSAF5M10HM3/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SS24FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512-SS24FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D40,D51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingbright</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP2012EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-AP2012EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT2012YC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-APT2012YC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT2012SGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-APT2012SGC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT2012QBC/D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">604-APT2012QBC/D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P-MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PowerPAK1212-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SISS27DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78-SISS27DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alternative: SISS27ADN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPN-Transistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC846BLT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-BC846BLT3G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-MOSFET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIS488DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78-SIS488DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">better: SIS862DN-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switching regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFN14 4x3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Richtek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT7259GQW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1028-1199-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSOP-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Instruments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS54340DDAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-TPS54340DDAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QFN-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semtech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS30041-M033QFNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">947-TS30041-M033QFNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQFP-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32F401VBT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-STM32F401VBT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2xOR-Gate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VSSOP-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74LVC2G32DC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-SN74LVC2G32DCUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M74VHC1G126DTT1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-M74VHC1G126DTT1G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QFN-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invensense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICM-20689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">410-ICM-20689</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U44,U45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motordriver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSON-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRV8835DSSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-DRV8835DSSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pushbutton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FSM2JSMASTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">506-FSM2JSMASTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combined (preffered)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speaker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS-PRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPEG158-P5H</t>
   </si>
   <si>
     <t xml:space="preserve">RS-Components</t>
-  </si>
-  <si>
-    <t xml:space="preserve">801-5347</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2n4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM1885C1H242JA01D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">815-1474</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM0335C1E220JA01D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81-GRM0335C1E220JA1D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C33, C34, C52, C54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22µ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM188R60J226ME15D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81-GRM188R60J226ME5D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL60XX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coilcraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL6030-222MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">994-XAL6030-222MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4µ7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL4030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL4030-472MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">994-XAL4030-472MEB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bourns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRN4018TA-4R7M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">652-SRN4018TA-4R7M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS160808-1R0K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">652-CS160808-1R0K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FB1, FB2, FB3, FB4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferrite Bead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLM31KN471SN1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81-BLM31KN471SN1L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z-Diode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD323-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ON Semiconductor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MM3Z18VST1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">863-MM3Z18VST1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD323F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MM3Z24VB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">512-MM3Z24VB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3,D44,D45,D46,D47,D48,D49,D50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3V6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fairchild</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDZ3V6ASF-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">621-DDZ3V6ASF-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5V2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD-123-F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nexperia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NZH5V1B,115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">771-NZH5V1B-115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schottky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DO-221AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSSAF5M10HM3/H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78-VSSAF5M10HM3/H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOD-123-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SS24FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">512-SS24FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D40,D51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kingbright</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP2012EC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-AP2012EC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yellow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APT2012YC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-APT2012YC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APT2012SGC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-APT2012SGC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APT2012QBC/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">604-APT2012QBC/D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-MOSFET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PowerPAK1212-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SISS27DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78-SISS27DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alternative: SISS27ADN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPN-Transistor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT23-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BC846BLT3G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">863-BC846BLT3G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-MOSFET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIS488DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78-SIS488DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">better: SIS862DN-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switching regulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DFN14 4x3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Richtek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT7259GQW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1028-1199-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSOP-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Texas Instruments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TPS54340DDAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">595-TPS54340DDAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QFN-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semtech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS30041-M033QFNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">947-TS30041-M033QFNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microcontroller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LQFP-100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F401VBT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">511-STM32F401VBT6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2xOR-Gate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VSSOP-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74LVC2G32DC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">816-8820</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buffer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M74VHC1G126DTT1G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">805-1494</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QFN-24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invensense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICM-20689</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1428-1059-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U44,U45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motordriver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WSON-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRV8835DSSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">813-6485</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pushbutton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FSM2JSMASTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">131-4776</t>
-  </si>
-  <si>
-    <t xml:space="preserve">combined (preffered)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speaker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS-PRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPEG158-P5H</t>
   </si>
   <si>
     <t xml:space="preserve">771-6910</t>
@@ -887,7 +902,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -930,12 +945,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1018,26 +1027,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1070,25 +1079,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:50"/>
+  <dimension ref="1:51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J42" activeCellId="0" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="71.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="73.5910931174089"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="6.21457489878543"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2154,7 +2163,7 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -2172,7 +2181,7 @@
       <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -2185,8 +2194,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="6" t="n">
@@ -2211,7 +2220,7 @@
       <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -2228,8 +2237,8 @@
       <c r="T4" s="0"/>
       <c r="U4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="6" t="n">
@@ -2248,13 +2257,13 @@
       <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -2271,8 +2280,8 @@
       <c r="T5" s="0"/>
       <c r="U5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="6" t="n">
@@ -2291,13 +2300,13 @@
       <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="10" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="10" t="s">
         <v>31</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -2314,8 +2323,8 @@
       <c r="T6" s="0"/>
       <c r="U6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+    <row r="7" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="6" t="n">
@@ -2340,7 +2349,7 @@
       <c r="I7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="10" t="s">
         <v>35</v>
       </c>
       <c r="K7" s="2" t="s">
@@ -2357,8 +2366,8 @@
       <c r="T7" s="0"/>
       <c r="U7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="6" t="n">
@@ -2383,7 +2392,7 @@
       <c r="I8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>38</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -2400,18 +2409,38 @@
       <c r="T8" s="0"/>
       <c r="U8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+    <row r="9" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L9" s="0"/>
       <c r="M9" s="0"/>
       <c r="N9" s="0"/>
@@ -2424,39 +2453,17 @@
       <c r="U9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>1206</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A10" s="11"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
       <c r="N10" s="0"/>
@@ -2469,35 +2476,35 @@
       <c r="U10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="5" t="n">
+        <v>1206</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="H11" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>19</v>
@@ -2514,35 +2521,35 @@
       <c r="U11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>19</v>
@@ -2559,26 +2566,26 @@
       <c r="U12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>57</v>
+      <c r="A13" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>3</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>59</v>
@@ -2604,32 +2611,32 @@
       <c r="U13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="9" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="6" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>66</v>
@@ -2649,32 +2656,32 @@
       <c r="U14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B15" s="6" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>69</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>70</v>
@@ -2694,35 +2701,35 @@
       <c r="U15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>72</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>19</v>
@@ -2739,35 +2746,35 @@
       <c r="U16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>75</v>
+      <c r="A17" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="B17" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>77</v>
+        <v>47</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>19</v>
@@ -2784,16 +2791,39 @@
       <c r="U17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="A18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
@@ -2806,33 +2836,16 @@
       <c r="U18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="A19" s="11"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
@@ -2846,23 +2859,24 @@
       <c r="U19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
-        <v>85</v>
+      <c r="A20" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="0"/>
+      <c r="F20" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="H20" s="5" t="s">
         <v>88</v>
@@ -2886,25 +2900,26 @@
       <c r="U20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="9" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>86</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E21" s="0"/>
       <c r="F21" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I21" s="5" t="s">
@@ -2925,37 +2940,36 @@
       <c r="T21" s="0"/>
       <c r="U21" s="0"/>
     </row>
-    <row r="22" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E22" s="0"/>
       <c r="F22" s="5" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="K22" s="7"/>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
@@ -2967,16 +2981,38 @@
       <c r="T22" s="0"/>
       <c r="U22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="0"/>
+      <c r="F23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
@@ -2988,40 +3024,18 @@
       <c r="T23" s="0"/>
       <c r="U23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="0"/>
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -3033,17 +3047,40 @@
       <c r="T24" s="0"/>
       <c r="U24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="7"/>
+    <row r="25" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -3056,36 +3093,16 @@
       <c r="U25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B26" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A26" s="9"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="7"/>
       <c r="L26" s="0"/>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -3098,161 +3115,171 @@
       <c r="U26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="5" t="s">
         <v>116</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
+      <c r="L27" s="0"/>
+      <c r="M27" s="0"/>
+      <c r="N27" s="0"/>
+      <c r="O27" s="0"/>
+      <c r="P27" s="0"/>
+      <c r="Q27" s="0"/>
+      <c r="R27" s="0"/>
+      <c r="S27" s="0"/>
+      <c r="T27" s="0"/>
+      <c r="U27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" s="5" t="s">
+      <c r="B28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>118</v>
       </c>
       <c r="F28" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="2" t="s">
         <v>121</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="B29" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="F30" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="G30" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="H30" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>135</v>
+      <c r="A31" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>138</v>
@@ -3267,56 +3294,56 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
         <v>140</v>
       </c>
       <c r="B32" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="F32" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
+    <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="G33" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>149</v>
@@ -3332,23 +3359,23 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="9" t="s">
         <v>151</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>152</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>153</v>
@@ -3363,403 +3390,445 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
         <v>155</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>156</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H35" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>157</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="J35" s="5" t="s">
         <v>158</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
+    <row r="36" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B37" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="F37" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>164</v>
-      </c>
+      <c r="A37" s="11"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>165</v>
+      <c r="A38" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="B38" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="F38" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="F38" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>19</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B39" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="5"/>
+      <c r="F39" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D39" s="7"/>
-      <c r="F39" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H39" s="8" t="s">
+      <c r="G39" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H39" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="5" t="s">
         <v>173</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>174</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
+      <c r="A40" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="F40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B41" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>176</v>
-      </c>
+      <c r="A41" s="9"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="F41" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>182</v>
+      <c r="A42" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="B42" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="F42" s="5" t="s">
+      <c r="F42" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="G42" s="5" t="s">
+      <c r="I42" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="J42" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>186</v>
-      </c>
+      <c r="K42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
-        <v>187</v>
+      <c r="A43" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="B43" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D43" s="5"/>
       <c r="F43" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G43" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="H43" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>190</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>191</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="K43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>192</v>
+      <c r="A44" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="B44" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="D44" s="5"/>
       <c r="F44" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H44" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>197</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="K44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
-        <v>198</v>
+      <c r="A45" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="B45" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D45" s="5"/>
       <c r="F45" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H45" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="G45" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H45" s="5" t="s">
+      <c r="I45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>202</v>
-      </c>
+      <c r="K45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>203</v>
+      <c r="A46" s="9" t="s">
+        <v>202</v>
       </c>
       <c r="B46" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C46" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D46" s="5"/>
+      <c r="F46" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="D46" s="5"/>
-      <c r="F46" s="10" t="s">
+      <c r="G46" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H46" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H46" s="5" t="s">
+      <c r="I46" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J46" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="I46" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>207</v>
-      </c>
+      <c r="K46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
-        <v>208</v>
+      <c r="A47" s="9" t="s">
+        <v>207</v>
       </c>
       <c r="B47" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D47" s="5"/>
       <c r="F47" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H47" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="I47" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="H47" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>213</v>
-      </c>
+      <c r="K47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>214</v>
+      <c r="A48" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="B48" s="6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D48" s="5"/>
       <c r="F48" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H48" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H48" s="5" t="s">
+      <c r="I48" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>218</v>
-      </c>
+      <c r="K48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7"/>
+      <c r="A49" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B49" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="F49" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="K49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B50" s="6" t="n">
+      <c r="A50" s="11"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="0"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B51" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="K50" s="14" t="s">
+      <c r="C51" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="K51" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3782,20 +3851,20 @@
   <dimension ref="1:18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="2" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="7.71255060728745"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="9.10526315789474"/>
   </cols>
@@ -3811,7 +3880,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -3832,7 +3901,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4862,29 +4931,29 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>226</v>
+      <c r="A3" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="0"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>65</v>
+        <v>234</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -5916,17 +5985,17 @@
     </row>
     <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="2" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="2"/>
@@ -5934,26 +6003,26 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
       <c r="F6" s="0"/>
       <c r="K6" s="2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="N6" s="0"/>
       <c r="O6" s="0"/>
@@ -6969,21 +7038,21 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="E7" s="0"/>
       <c r="F7" s="0"/>
       <c r="K7" s="2" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="N7" s="0"/>
       <c r="O7" s="0"/>
@@ -7999,19 +8068,19 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="0"/>
       <c r="F8" s="0"/>
       <c r="K8" s="2" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="N8" s="0"/>
       <c r="O8" s="0"/>
@@ -9027,21 +9096,21 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="E9" s="0"/>
       <c r="F9" s="0"/>
       <c r="K9" s="2" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="N9" s="0"/>
       <c r="O9" s="0"/>
@@ -10057,157 +10126,157 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="K10" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
       <c r="K11" s="2" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B12" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
       <c r="K12" s="2" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B13" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
       <c r="K13" s="2" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
       <c r="F14" s="0"/>
       <c r="K14" s="2" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
       <c r="K15" s="2" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="B16" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
       <c r="K16" s="2" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="K17" s="2" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="B18" s="2" t="n">
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
       <c r="K18" s="2" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -10234,7 +10303,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10246,9 +10315,9 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="2" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="2" width="9.10526315789474"/>
   </cols>
@@ -10285,13 +10354,13 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>1</v>
@@ -10300,25 +10369,25 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="K3" s="5"/>
     </row>
@@ -10327,34 +10396,34 @@
     </row>
     <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="K5" s="5"/>
     </row>
@@ -10363,20 +10432,20 @@
     </row>
     <row r="7" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="17" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -10399,17 +10468,17 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="17" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="1"/>
@@ -10417,26 +10486,26 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="2" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="F10" s="17"/>
       <c r="K10" s="2" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>